<commit_message>
Actualizando planilla con complementos posteriores a la entrega
</commit_message>
<xml_diff>
--- a/df_total_e4.xlsx
+++ b/df_total_e4.xlsx
@@ -9543,7 +9543,7 @@
 - El espacio que estás considerando para tu sección por fachada es insuficiente para lo que necesitas.
 - El 3D q presentas no corresponde a lo que estás diseñando. Esto es grave!
 - Debes tener intenciones para diagramar más claras y efectivas. Esto lo podremos revisar en una próxima asesoría, pero por lo pronto, inclinar de manera aleatoria dibujos cuya representación técnica surge de una vista ortogonal (ej: planta, sección y fachada) no le aporta valor a tu memoria y antes confunde.
-La nota general para esta entrega es 2.5.</t>
+La nota general para esta entrega es 3,8.</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
@@ -9664,12 +9664,12 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -9679,12 +9679,12 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>E4.Arg_NA</t>
+          <t>E4.Arg_A</t>
         </is>
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Argumenta las decisiones de diseño de manera sólida y coherente, basándose en fundamentos disciplinares y un profundo conocimiento del usuario. Las decisiones están bien justificadas y son consistentes.</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
@@ -10738,7 +10738,7 @@
 Comentario personal representación:
 - Debes considerar las escalas de los planos solicitados: entregas una planta en 1:200 y necesitabas presentarla en 1:50. Al no representar en dichas escalas, no podemos ver el detalle de ciertos aspectos del dibujo que solo se ven a ese tamaño.
 - Le das mucha más importancia al 3D en el espacio total disponible para la memoria, pero en contra del espacio que requieres para la planta en un nivel.
-La nota general para esta entrega es 3,1.</t>
+La nota general para esta entrega es 4,4.</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
@@ -10859,12 +10859,12 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E220" t="inlineStr">
@@ -10874,12 +10874,12 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>E4.Arg_NA</t>
+          <t>E4.Arg_A</t>
         </is>
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Argumenta las decisiones de diseño de manera sólida y coherente, basándose en fundamentos disciplinares y un profundo conocimiento del usuario. Las decisiones están bien justificadas y son consistentes.</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
@@ -31053,8 +31053,8 @@
       </c>
       <c r="G642" t="inlineStr">
         <is>
-          <t>No entregaste y por tanto no tenemos comentarios particulares sobre tu proyecto a nivel funcional, ni de representación. Si quieres alcanzar las competencias que requieres para aprobar este taller, es necesario que eleves tu nivel de producción y sincronización con los tiempos establecidos para el curso.
-La nota general para esta entrega es 2.5.</t>
+          <t>Al revisar lo que entregaste en una fecha posterior, debido al apoyo que le diste de manera oportuna a tu compañera, hemos ajustado tu evaluación. Aún es necesario que eleves tu nivel de reflexión espacial y producción para los productos que debes presentar en la entrega final.
+La nota general para esta entrega es 4.3.</t>
         </is>
       </c>
       <c r="H642" t="inlineStr">
@@ -31081,12 +31081,12 @@
       </c>
       <c r="C643" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="D643" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E643" t="inlineStr">
@@ -31096,12 +31096,12 @@
       </c>
       <c r="F643" t="inlineStr">
         <is>
-          <t>E4.Func_NA</t>
+          <t>E4.Func_B</t>
         </is>
       </c>
       <c r="G643" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Aplica estrategias de composición formal en una vivienda con algunas inconsistencias en la integración de las variables propuestas para el ejercicio. El proyecto presenta algunas debilidades en su función y/o en su resolución técnica.</t>
         </is>
       </c>
       <c r="H643" t="inlineStr">
@@ -31128,12 +31128,12 @@
       </c>
       <c r="C644" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="D644" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E644" t="inlineStr">
@@ -31143,12 +31143,12 @@
       </c>
       <c r="F644" t="inlineStr">
         <is>
-          <t>E4.Rep_NA</t>
+          <t>E4.Rep_B</t>
         </is>
       </c>
       <c r="G644" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Utiliza recursos verbales y gráficos en 2 y 3 dimensiones para representar y comunicar el proyecto, aunque con algunas inconsistencias en la coherencia y la efectividad de la comunicación. La presentación es generalmente clara, pero ciertos aspectos claves del proyecto no están suficientemente desarrollados o explicados.</t>
         </is>
       </c>
       <c r="H644" t="inlineStr">
@@ -40631,8 +40631,10 @@
 - Revisa escala de planos que presentas: para la próxima semana, vuelve a traer impresas 3 plantas en Esc-1:50 para que podamos resolver detalles funcionales (no incluyas detalles de ambientación de la memoria: solo planos).
 - Revisa intenciones al representar y la cantidad de cosas que añades.
 - Aumenta el tamaño del cuadro de áreas para poder ver su información.
+Comentario personal "argumentación":
+- Has subido la historia de tu familia posterior a la entrega, pero lo has hecho a manera de fotografía desde tu bitácota y les habíamos solicitado que digitalizaran dicho texto (ej: word)
 Nota general:
-Tu nota general es 3.1 y por tener 0.5 acumulado de la entrega previa, esta sube a 3.6</t>
+Tu nota general es 3.9 y por tener 0.5 acumulado de la entrega previa, esta sube a 4,4</t>
         </is>
       </c>
       <c r="H842" t="inlineStr">
@@ -40753,12 +40755,12 @@
       </c>
       <c r="C845" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="D845" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E845" t="inlineStr">
@@ -40768,12 +40770,12 @@
       </c>
       <c r="F845" t="inlineStr">
         <is>
-          <t>E4.Arg_NA</t>
+          <t>E4.Arg_B</t>
         </is>
       </c>
       <c r="G845" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Presenta una argumentación aceptable para las decisiones de diseño, pero con algunas inconsistencias o falta de profundidad en los fundamentos disciplinares o el conocimiento del usuario.</t>
         </is>
       </c>
       <c r="H845" t="inlineStr">
@@ -41816,8 +41818,8 @@
       </c>
       <c r="G867" t="inlineStr">
         <is>
-          <t>No entregaste y por tanto no tenemos comentarios particulares sobre tu proyecto a nivel funcional, de representación ni argumentativo (tampoco subiste la historia de tu familia, cuando lo solicitamos semanas atrás). Si quieres alcanzar las competencias que requieres para aprobar este taller, es necesario que eleves tu nivel de producción y sincronización con los tiempos establecidos para el curso.
-La nota general para esta entrega es 1.3.</t>
+          <t>Al revisar lo que entregaste en una fecha posterior, debido a la situación difícil que viviste, hemos ajustado tu evaluación. Reconocemos tu valor para continuar y la capacidad para reintegrarte a las actividades del taller. Aún es necesario que eleves tu nivel de reflexión espacial y producción para los productos que debes presentar en la entrega final.
+La nota general para esta entrega es 4.3</t>
         </is>
       </c>
       <c r="H867" t="inlineStr">
@@ -41844,12 +41846,12 @@
       </c>
       <c r="C868" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="D868" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E868" t="inlineStr">
@@ -41859,12 +41861,12 @@
       </c>
       <c r="F868" t="inlineStr">
         <is>
-          <t>E4.Func_NA</t>
+          <t>E4.Func_B</t>
         </is>
       </c>
       <c r="G868" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Aplica estrategias de composición formal en una vivienda con algunas inconsistencias en la integración de las variables propuestas para el ejercicio. El proyecto presenta algunas debilidades en su función y/o en su resolución técnica.</t>
         </is>
       </c>
       <c r="H868" t="inlineStr">
@@ -41891,12 +41893,12 @@
       </c>
       <c r="C869" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="D869" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E869" t="inlineStr">
@@ -41906,12 +41908,12 @@
       </c>
       <c r="F869" t="inlineStr">
         <is>
-          <t>E4.Rep_NA</t>
+          <t>E4.Rep_B</t>
         </is>
       </c>
       <c r="G869" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Utiliza recursos verbales y gráficos en 2 y 3 dimensiones para representar y comunicar el proyecto, aunque con algunas inconsistencias en la coherencia y la efectividad de la comunicación. La presentación es generalmente clara, pero ciertos aspectos claves del proyecto no están suficientemente desarrollados o explicados.</t>
         </is>
       </c>
       <c r="H869" t="inlineStr">
@@ -41938,12 +41940,12 @@
       </c>
       <c r="C870" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="D870" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E870" t="inlineStr">
@@ -41953,12 +41955,12 @@
       </c>
       <c r="F870" t="inlineStr">
         <is>
-          <t>E4.Arg_NA</t>
+          <t>E4.Arg_A</t>
         </is>
       </c>
       <c r="G870" t="inlineStr">
         <is>
-          <t>...</t>
+          <t>Argumenta las decisiones de diseño de manera sólida y coherente, basándose en fundamentos disciplinares y un profundo conocimiento del usuario. Las decisiones están bien justificadas y son consistentes.</t>
         </is>
       </c>
       <c r="H870" t="inlineStr">

</xml_diff>